<commit_message>
TopKnee Update with Nut and Bolts Setup
05_05_Knee_top part file was updated with the nut and bolt setup for connecting to the femur

Working on updating the BOM excel file with new parts being ordered. Nuts, washers, lock nuts
</commit_message>
<xml_diff>
--- a/Solid Models/00_Bipedal_Robot/11_BOM_Robot/00_BOMSheet_Excel.xlsx
+++ b/Solid Models/00_Bipedal_Robot/11_BOM_Robot/00_BOMSheet_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\AARL\Github\Bipedal_Robot\Solid Models\00_Bipedal_Robot\11_BOM_Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14ADAF9-64AB-458B-B427-045200FCCD61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612621AA-F326-4D10-8A9E-C841BF45A3C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{94461439-9888-4703-AD57-24F63FAB8AC4}"/>
+    <workbookView xWindow="28680" yWindow="-2400" windowWidth="29040" windowHeight="17640" xr2:uid="{94461439-9888-4703-AD57-24F63FAB8AC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t xml:space="preserve">Part Name </t>
   </si>
@@ -94,13 +94,55 @@
   </si>
   <si>
     <t>https://www.mcmaster.com/97042A216/</t>
+  </si>
+  <si>
+    <t>Nut</t>
+  </si>
+  <si>
+    <t>Mcmaster</t>
+  </si>
+  <si>
+    <t>Nut to replace Brass inserts</t>
+  </si>
+  <si>
+    <t>95462A029</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/95462A029/</t>
+  </si>
+  <si>
+    <t>lock nut</t>
+  </si>
+  <si>
+    <t>to keep bolt in place</t>
+  </si>
+  <si>
+    <t>91102A750</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/91102A750/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">washer </t>
+  </si>
+  <si>
+    <t>92141A029</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92141A029/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>What we need to buy for a new connection design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +154,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,10 +293,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -252,8 +309,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -566,23 +630,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170F1F73-466A-43CC-9378-1D56403BA97A}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.86328125" customWidth="1"/>
-    <col min="5" max="5" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -602,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -615,14 +679,14 @@
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -635,14 +699,14 @@
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -655,14 +719,17 @@
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -675,175 +742,245 @@
       <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>10</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>11</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>12</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="12"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E15" s="12"/>
+      <c r="F15" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>14</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="12"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>15</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>16</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>17</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="E19" s="12"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>18</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="E20" s="12"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>19</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="E21" s="12"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>20</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="10"/>
     </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" xr:uid="{1B40CD0D-BF7D-4909-944C-5E87CEEDC38A}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{63FC7DBA-7B3F-4B8D-B1F7-309279B5901E}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{F6AD0294-5E93-4599-B85C-E02D5705A212}"/>
+    <hyperlink ref="F25" r:id="rId4" xr:uid="{65210273-1118-465D-9EFB-F0D2EB160BDF}"/>
+    <hyperlink ref="F26" r:id="rId5" xr:uid="{F97E09F3-1DCE-4705-916C-CE3B3900A3EE}"/>
+    <hyperlink ref="F27" r:id="rId6" xr:uid="{0D9D11A9-DE8E-450E-A9FC-4E2E6C8AB084}"/>
+    <hyperlink ref="F3" r:id="rId7" xr:uid="{E8D1CAE5-D00E-4BA9-8050-09EE5978A43C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>